<commit_message>
Add a lot of functionality
</commit_message>
<xml_diff>
--- a/analysis/tables/tables_original_versions/function_weights.xlsx
+++ b/analysis/tables/tables_original_versions/function_weights.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f7c04bbdd3c4e0fe/Bureaublad/WEB/GitHubSync/Vipertje/analysis/tables/tables_original_versions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="13_ncr:1_{CACBE3BE-6A37-41FB-8845-814A01E82F73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8284675F-31A5-402C-8508-759C0608CC98}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="13_ncr:1_{CACBE3BE-6A37-41FB-8845-814A01E82F73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9D1CBD3F-A871-4460-BCB7-127123A2DB21}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="30">
   <si>
     <t>function</t>
   </si>
@@ -57,12 +57,6 @@
     <t>student_housing</t>
   </si>
   <si>
-    <t>carparking_private</t>
-  </si>
-  <si>
-    <t>bikeparking_private</t>
-  </si>
-  <si>
     <t>care_centre</t>
   </si>
   <si>
@@ -84,18 +78,9 @@
     <t>starter_housing</t>
   </si>
   <si>
-    <t>city_garden</t>
-  </si>
-  <si>
     <t>elderly_housing</t>
   </si>
   <si>
-    <t>carparking_public</t>
-  </si>
-  <si>
-    <t>bikeparking_public</t>
-  </si>
-  <si>
     <t>str</t>
   </si>
   <si>
@@ -127,6 +112,9 @@
   </si>
   <si>
     <t>inv_height_analysis</t>
+  </si>
+  <si>
+    <t>laundry_room</t>
   </si>
 </sst>
 </file>
@@ -572,10 +560,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -604,10 +592,10 @@
         <v>6</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>1</v>
@@ -615,28 +603,28 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -644,7 +632,7 @@
         <v>9</v>
       </c>
       <c r="B3" s="3">
-        <v>1000</v>
+        <v>10000</v>
       </c>
       <c r="C3" s="4">
         <v>0</v>
@@ -653,7 +641,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="F3" s="4">
         <v>0</v>
@@ -662,15 +650,15 @@
         <v>1</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B4" s="3">
-        <v>1200</v>
+        <v>12000</v>
       </c>
       <c r="C4" s="4">
         <v>0</v>
@@ -679,7 +667,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="F4" s="4">
         <v>1</v>
@@ -688,15 +676,15 @@
         <v>0</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B5" s="3">
-        <v>1300</v>
+        <v>13000</v>
       </c>
       <c r="C5" s="4">
         <v>1000</v>
@@ -705,33 +693,33 @@
         <v>1</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B6" s="3">
-        <v>16000</v>
+        <v>600</v>
       </c>
       <c r="C6" s="4">
         <v>0</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6" s="4">
-        <v>0</v>
+        <v>26</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="F6" s="4">
         <v>0</v>
@@ -739,25 +727,25 @@
       <c r="G6" s="4">
         <v>1</v>
       </c>
-      <c r="H6" s="4">
-        <v>0</v>
+      <c r="H6" s="4" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="B7" s="3">
-        <v>2533</v>
+        <v>200</v>
       </c>
       <c r="C7" s="4">
-        <v>0</v>
+        <v>240</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" s="4">
-        <v>0</v>
+        <v>22</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="F7" s="4">
         <v>0</v>
@@ -765,26 +753,25 @@
       <c r="G7" s="4">
         <v>1</v>
       </c>
-      <c r="H7" s="4">
-        <v>0</v>
+      <c r="H7" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="B8" s="3">
-        <f>(SUM(B11+B10+B13+B14+B17)/200)*4</f>
-        <v>39.799999999999997</v>
+        <v>230</v>
       </c>
       <c r="C8" s="4">
         <v>0</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E8" s="4">
-        <v>0</v>
+        <v>22</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="F8" s="4">
         <v>0</v>
@@ -792,26 +779,25 @@
       <c r="G8" s="4">
         <v>1</v>
       </c>
-      <c r="H8" s="4">
-        <v>0</v>
+      <c r="H8" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="3">
+        <v>60</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="3">
-        <f>(SUM(B11+B10+B13+B14+B17)/200)*10</f>
-        <v>99.5</v>
-      </c>
-      <c r="C9" s="4">
-        <v>0</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E9" s="4">
-        <v>0</v>
+      <c r="E9" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="F9" s="4">
         <v>0</v>
@@ -819,25 +805,25 @@
       <c r="G9" s="4">
         <v>1</v>
       </c>
-      <c r="H9" s="4">
-        <v>0</v>
+      <c r="H9" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B10" s="3">
-        <v>600</v>
+        <v>550</v>
       </c>
       <c r="C10" s="4">
         <v>0</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="F10" s="4">
         <v>0</v>
@@ -845,25 +831,25 @@
       <c r="G10" s="4">
         <v>1</v>
       </c>
-      <c r="H10" s="4" t="s">
-        <v>30</v>
+      <c r="H10" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B11" s="3">
-        <v>200</v>
+        <v>60</v>
       </c>
       <c r="C11" s="4">
-        <v>240</v>
+        <v>0</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F11" s="4">
         <v>0</v>
@@ -872,102 +858,102 @@
         <v>1</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B12" s="3">
-        <v>5500</v>
+        <v>900</v>
       </c>
       <c r="C12" s="4">
         <v>0</v>
       </c>
-      <c r="D12" s="4">
-        <v>1</v>
-      </c>
-      <c r="E12" s="4">
-        <v>1</v>
-      </c>
-      <c r="F12" s="4" t="s">
+      <c r="D12" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="G12" s="4" t="s">
-        <v>26</v>
+      <c r="F12" s="4">
+        <v>0</v>
+      </c>
+      <c r="G12" s="4">
+        <v>1</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B13" s="3">
-        <v>230</v>
+        <v>500</v>
       </c>
       <c r="C13" s="4">
         <v>0</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="F13" s="4">
         <v>0</v>
       </c>
-      <c r="G13" s="4">
-        <v>1</v>
+      <c r="G13" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B14" s="3">
-        <v>60</v>
+        <v>300</v>
       </c>
       <c r="C14" s="4">
         <v>0</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="F14" s="4">
         <v>0</v>
       </c>
-      <c r="G14" s="4">
-        <v>1</v>
+      <c r="G14" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="B15" s="3">
-        <v>550</v>
+        <v>100</v>
       </c>
       <c r="C15" s="4">
         <v>0</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>30</v>
+        <v>21</v>
+      </c>
+      <c r="E15" s="4">
+        <v>0</v>
       </c>
       <c r="F15" s="4">
         <v>0</v>
@@ -976,112 +962,206 @@
         <v>1</v>
       </c>
       <c r="H15" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" s="3">
-        <v>60</v>
-      </c>
-      <c r="C16" s="4">
-        <v>0</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F16" s="4">
-        <v>0</v>
-      </c>
-      <c r="G16" s="4">
-        <v>1</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="3">
-        <v>900</v>
-      </c>
-      <c r="C17" s="4">
-        <v>0</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F17" s="4">
-        <v>0</v>
-      </c>
-      <c r="G17" s="4">
-        <v>1</v>
-      </c>
-      <c r="H17" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="3">
-        <v>500</v>
-      </c>
-      <c r="C18" s="4">
-        <v>0</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F18" s="4">
-        <v>0</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="H18" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="3">
-        <v>300</v>
-      </c>
-      <c r="C19" s="4">
-        <v>0</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F19" s="4">
-        <v>0</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>28</v>
-      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="3"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="3"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="3"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="3"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="3"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="3"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="3"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="3"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="3"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="3"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="3"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B28" s="3"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="3"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B30" s="3"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B31" s="3"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B32" s="3"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B33" s="3"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B34" s="3"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B35" s="3"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B36" s="3"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B37" s="3"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>